<commit_message>
parsing command line arguments
</commit_message>
<xml_diff>
--- a/test_files/locators.xlsx
+++ b/test_files/locators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidyashree M C\demo_project\POM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidyashree M C\demo_project\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>login_link</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>button-1.login-button</t>
+  </si>
+  <si>
+    <t>logout_link</t>
+  </si>
+  <si>
+    <t>Log out</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +453,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>